<commit_message>
LEDON weg: gleiches Bit wie STOP_ON !!!
</commit_message>
<xml_diff>
--- a/mixing.xlsx
+++ b/mixing.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruediheimlicher/Documents/Programming/RC/RC_22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6364C97-4E47-B34C-AF8B-2F5FAFEDABFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1864AB7-6BA2-D141-A22C-DCA2739A58F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5660" yWindow="3680" windowWidth="27640" windowHeight="16860" xr2:uid="{6C1C1D41-1015-F54E-8F28-A20310550484}"/>
+    <workbookView xWindow="9600" yWindow="23540" windowWidth="19700" windowHeight="13280" activeTab="1" xr2:uid="{6C1C1D41-1015-F54E-8F28-A20310550484}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="akku" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="31">
   <si>
     <t xml:space="preserve">mixindex: 0 kanalwerta : </t>
   </si>
@@ -84,6 +86,51 @@
   <si>
     <t>kanalb</t>
   </si>
+  <si>
+    <t>MINSPANNUNG</t>
+  </si>
+  <si>
+    <t>MAXSPANNUNG</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>balkenhoehe</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">akkuwert: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> masterstatus: 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> masterstatus: 0</t>
+  </si>
+  <si>
+    <t>bat f</t>
+  </si>
+  <si>
+    <t>bat i</t>
+  </si>
+  <si>
+    <t>Faktor</t>
+  </si>
+  <si>
+    <t>grenze</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>7-full</t>
+  </si>
+  <si>
+    <t>full &lt; grenze - 1</t>
+  </si>
 </sst>
 </file>
 
@@ -98,12 +145,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -118,8 +171,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2565,6 +2621,1051 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>akku!$C$7:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0678-3446-8634-521A4F3105D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>akku!$D$7:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0678-3446-8634-521A4F3105D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>akku!$G$7:$G$14</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0678-3446-8634-521A4F3105D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="732182912"/>
+        <c:axId val="732183312"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="732182912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="732183312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="732183312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="732182912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9247594050743664E-2"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.86486351706036746"/>
+          <c:h val="0.74403579760863225"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle3!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bat i</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle3!$B$2:$B$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>1942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1945</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1954</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1943</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1922</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1854</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1839</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1792</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1751</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1751</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1751</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1751</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1746</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1745</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1746</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1760</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1835</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1894</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1924</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1956</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2072</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2118</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2129</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2210</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2275</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2304</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2324</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2363</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2383</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2385</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2397</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2382</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2355</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2336</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2275</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2246</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2164</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2164</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2151</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2209</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2163</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2164</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2149</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2164</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2164</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle3!$D$2:$D$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="53"/>
+                <c:pt idx="0">
+                  <c:v>647</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>648</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>613</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>583</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>581</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>582</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>586</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>611</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>631</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>641</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>706</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>709</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>774</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>787</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>794</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>795</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>799</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>794</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>785</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>778</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>758</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>748</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>736</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>721</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>721</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A508-8946-8A59-13DD7BD24613}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="749592688"/>
+        <c:axId val="749729360"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="749592688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1700"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="749729360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="749729360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="749592688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2606,6 +3707,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3677,6 +4858,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3746,6 +5959,88 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA78E96-DDBA-FF43-8701-4B4A63BA6227}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC50007-E5CB-D844-9563-FC508C354476}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4053,7 +6348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4349273B-762E-E049-8E2F-91927F78DF30}">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
@@ -9363,4 +11658,1498 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314B67F5-5559-1843-97D9-9100CD76D128}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <f>D1</f>
+        <v>620</v>
+      </c>
+      <c r="C7" s="1">
+        <f>(B7-$D$1)*$D$3/($D$2-$D$1)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>INT(C7/8)</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>IF(D7&lt;$D$4-1,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>7-D7</f>
+        <v>7</v>
+      </c>
+      <c r="G7" s="1">
+        <f>1+INT(C7/8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <f>B7+$A$7</f>
+        <v>630</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" ref="C8:C25" si="0">(B8-$D$1)*$D$3/($D$2-$D$1)</f>
+        <v>2.9</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D25" si="1">INT(C8/8)</f>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E24" si="2">IF(D8&lt;$D$4-1,1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8:F25" si="3">7-D8</f>
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G25" si="4">1+INT(C8/8)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <f t="shared" ref="B9:B17" si="5">B8+$A$7</f>
+        <v>640</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <f t="shared" si="5"/>
+        <v>650</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="0"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <f t="shared" si="5"/>
+        <v>660</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>11.6</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <f t="shared" si="5"/>
+        <v>670</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>14.5</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <f t="shared" si="5"/>
+        <v>680</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <f t="shared" si="5"/>
+        <v>690</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="0"/>
+        <v>20.3</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f t="shared" si="5"/>
+        <v>700</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="0"/>
+        <v>23.2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f t="shared" si="5"/>
+        <v>710</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="0"/>
+        <v>26.1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" si="5"/>
+        <v>720</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" ref="B18:B23" si="6">B17+$A$7</f>
+        <v>730</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="0"/>
+        <v>31.9</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="6"/>
+        <v>740</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="0"/>
+        <v>34.799999999999997</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="6"/>
+        <v>750</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="0"/>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="6"/>
+        <v>760</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>40.6</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" si="6"/>
+        <v>770</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>43.5</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f t="shared" si="6"/>
+        <v>780</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>46.4</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <f t="shared" ref="B24:B25" si="7">B23+$A$7</f>
+        <v>790</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>49.3</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <f t="shared" si="7"/>
+        <v>800</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>52.2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C71A5C-EAA1-964E-936C-4FBE49CA9C6D}">
+  <dimension ref="A1:E54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>1942</v>
+      </c>
+      <c r="C2">
+        <v>6.47</v>
+      </c>
+      <c r="D2">
+        <v>647</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>1945</v>
+      </c>
+      <c r="C3">
+        <v>6.48</v>
+      </c>
+      <c r="D3">
+        <v>648</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>1954</v>
+      </c>
+      <c r="C4">
+        <v>6.51</v>
+      </c>
+      <c r="D4">
+        <v>651</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1944</v>
+      </c>
+      <c r="C5">
+        <v>6.48</v>
+      </c>
+      <c r="D5">
+        <v>648</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>1943</v>
+      </c>
+      <c r="C6">
+        <v>6.48</v>
+      </c>
+      <c r="D6">
+        <v>647</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>1944</v>
+      </c>
+      <c r="C7">
+        <v>6.48</v>
+      </c>
+      <c r="D7">
+        <v>648</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>1922</v>
+      </c>
+      <c r="C8">
+        <v>6.41</v>
+      </c>
+      <c r="D8">
+        <v>640</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9">
+        <v>1855</v>
+      </c>
+      <c r="C9">
+        <v>6.18</v>
+      </c>
+      <c r="D9">
+        <v>618</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1855</v>
+      </c>
+      <c r="C10">
+        <v>6.18</v>
+      </c>
+      <c r="D10">
+        <v>618</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>1854</v>
+      </c>
+      <c r="C11">
+        <v>6.18</v>
+      </c>
+      <c r="D11">
+        <v>618</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>1839</v>
+      </c>
+      <c r="C12">
+        <v>6.13</v>
+      </c>
+      <c r="D12">
+        <v>613</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13">
+        <v>1792</v>
+      </c>
+      <c r="C13">
+        <v>5.97</v>
+      </c>
+      <c r="D13">
+        <v>597</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>1751</v>
+      </c>
+      <c r="C14">
+        <v>5.84</v>
+      </c>
+      <c r="D14">
+        <v>583</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>1751</v>
+      </c>
+      <c r="C15">
+        <v>5.84</v>
+      </c>
+      <c r="D15">
+        <v>583</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>1750</v>
+      </c>
+      <c r="C16">
+        <v>5.83</v>
+      </c>
+      <c r="D16">
+        <v>583</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>1751</v>
+      </c>
+      <c r="C17">
+        <v>5.84</v>
+      </c>
+      <c r="D17">
+        <v>583</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>1751</v>
+      </c>
+      <c r="C18">
+        <v>5.84</v>
+      </c>
+      <c r="D18">
+        <v>583</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>1746</v>
+      </c>
+      <c r="C19">
+        <v>5.82</v>
+      </c>
+      <c r="D19">
+        <v>582</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>1745</v>
+      </c>
+      <c r="C20">
+        <v>5.82</v>
+      </c>
+      <c r="D20">
+        <v>581</v>
+      </c>
+      <c r="E20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>1746</v>
+      </c>
+      <c r="C21">
+        <v>5.82</v>
+      </c>
+      <c r="D21">
+        <v>582</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1760</v>
+      </c>
+      <c r="C22">
+        <v>5.87</v>
+      </c>
+      <c r="D22">
+        <v>586</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1810</v>
+      </c>
+      <c r="C23">
+        <v>6.03</v>
+      </c>
+      <c r="D23">
+        <v>603</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>1835</v>
+      </c>
+      <c r="C24">
+        <v>6.12</v>
+      </c>
+      <c r="D24">
+        <v>611</v>
+      </c>
+      <c r="E24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>1855</v>
+      </c>
+      <c r="C25">
+        <v>6.18</v>
+      </c>
+      <c r="D25">
+        <v>618</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26">
+        <v>1894</v>
+      </c>
+      <c r="C26">
+        <v>6.31</v>
+      </c>
+      <c r="D26">
+        <v>631</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27">
+        <v>1924</v>
+      </c>
+      <c r="C27">
+        <v>6.41</v>
+      </c>
+      <c r="D27">
+        <v>641</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28">
+        <v>1956</v>
+      </c>
+      <c r="C28">
+        <v>6.52</v>
+      </c>
+      <c r="D28">
+        <v>652</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <v>2041</v>
+      </c>
+      <c r="C29">
+        <v>6.8</v>
+      </c>
+      <c r="D29">
+        <v>680</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>2072</v>
+      </c>
+      <c r="C30">
+        <v>6.91</v>
+      </c>
+      <c r="D30">
+        <v>690</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>2118</v>
+      </c>
+      <c r="C31">
+        <v>7.06</v>
+      </c>
+      <c r="D31">
+        <v>706</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>2129</v>
+      </c>
+      <c r="C32">
+        <v>7.1</v>
+      </c>
+      <c r="D32">
+        <v>709</v>
+      </c>
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33">
+        <v>2210</v>
+      </c>
+      <c r="C33">
+        <v>7.37</v>
+      </c>
+      <c r="D33">
+        <v>736</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34">
+        <v>2275</v>
+      </c>
+      <c r="C34">
+        <v>7.58</v>
+      </c>
+      <c r="D34">
+        <v>758</v>
+      </c>
+      <c r="E34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>2304</v>
+      </c>
+      <c r="C35">
+        <v>7.68</v>
+      </c>
+      <c r="D35">
+        <v>768</v>
+      </c>
+      <c r="E35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>2324</v>
+      </c>
+      <c r="C36">
+        <v>7.75</v>
+      </c>
+      <c r="D36">
+        <v>774</v>
+      </c>
+      <c r="E36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <v>2363</v>
+      </c>
+      <c r="C37">
+        <v>7.88</v>
+      </c>
+      <c r="D37">
+        <v>787</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B38">
+        <v>2383</v>
+      </c>
+      <c r="C38">
+        <v>7.94</v>
+      </c>
+      <c r="D38">
+        <v>794</v>
+      </c>
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39">
+        <v>2385</v>
+      </c>
+      <c r="C39">
+        <v>7.95</v>
+      </c>
+      <c r="D39">
+        <v>795</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>2397</v>
+      </c>
+      <c r="C40">
+        <v>7.99</v>
+      </c>
+      <c r="D40">
+        <v>799</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41">
+        <v>2382</v>
+      </c>
+      <c r="C41">
+        <v>7.94</v>
+      </c>
+      <c r="D41">
+        <v>794</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42">
+        <v>2355</v>
+      </c>
+      <c r="C42">
+        <v>7.85</v>
+      </c>
+      <c r="D42">
+        <v>785</v>
+      </c>
+      <c r="E42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43">
+        <v>2336</v>
+      </c>
+      <c r="C43">
+        <v>7.79</v>
+      </c>
+      <c r="D43">
+        <v>778</v>
+      </c>
+      <c r="E43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B44">
+        <v>2275</v>
+      </c>
+      <c r="C44">
+        <v>7.58</v>
+      </c>
+      <c r="D44">
+        <v>758</v>
+      </c>
+      <c r="E44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45">
+        <v>2246</v>
+      </c>
+      <c r="C45">
+        <v>7.49</v>
+      </c>
+      <c r="D45">
+        <v>748</v>
+      </c>
+      <c r="E45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46">
+        <v>2164</v>
+      </c>
+      <c r="C46">
+        <v>7.21</v>
+      </c>
+      <c r="D46">
+        <v>721</v>
+      </c>
+      <c r="E46" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47">
+        <v>2164</v>
+      </c>
+      <c r="C47">
+        <v>7.21</v>
+      </c>
+      <c r="D47">
+        <v>721</v>
+      </c>
+      <c r="E47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>2151</v>
+      </c>
+      <c r="C48">
+        <v>7.17</v>
+      </c>
+      <c r="D48">
+        <v>717</v>
+      </c>
+      <c r="E48" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49">
+        <v>2209</v>
+      </c>
+      <c r="C49">
+        <v>7.36</v>
+      </c>
+      <c r="D49">
+        <v>736</v>
+      </c>
+      <c r="E49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50">
+        <v>2163</v>
+      </c>
+      <c r="C50">
+        <v>7.21</v>
+      </c>
+      <c r="D50">
+        <v>721</v>
+      </c>
+      <c r="E50" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>2164</v>
+      </c>
+      <c r="C51">
+        <v>7.21</v>
+      </c>
+      <c r="D51">
+        <v>721</v>
+      </c>
+      <c r="E51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52">
+        <v>2149</v>
+      </c>
+      <c r="C52">
+        <v>7.16</v>
+      </c>
+      <c r="D52">
+        <v>716</v>
+      </c>
+      <c r="E52" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53">
+        <v>2164</v>
+      </c>
+      <c r="C53">
+        <v>7.21</v>
+      </c>
+      <c r="D53">
+        <v>721</v>
+      </c>
+      <c r="E53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54">
+        <v>2164</v>
+      </c>
+      <c r="C54">
+        <v>7.21</v>
+      </c>
+      <c r="D54">
+        <v>721</v>
+      </c>
+      <c r="E54" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>